<commit_message>
updated search test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="76">
   <si>
     <t>API</t>
   </si>
@@ -130,7 +130,118 @@
     <t>?query=biotechnology +institute</t>
   </si>
   <si>
+    <t>S1_TC_T8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search for documents with multiple must contain worlds </t>
+  </si>
+  <si>
+    <t>?query=biotechnology +institute +cardiology</t>
+  </si>
+  <si>
+    <t>S1_TC_T9</t>
+  </si>
+  <si>
+    <t>search for documents which match the query with wild character.</t>
+  </si>
+  <si>
+    <t>?query=cardi*</t>
+  </si>
+  <si>
+    <t>S1_TC_T10</t>
+  </si>
+  <si>
+    <t>search for docuements with query and should not contain certain words (negative -)</t>
+  </si>
+  <si>
+    <t>?query=biotechnology -cardio</t>
+  </si>
+  <si>
+    <t>S1_TC_T11</t>
+  </si>
+  <si>
+    <t>Search for docuements with query and should not contain multiple words</t>
+  </si>
+  <si>
+    <t>?query=biotechnology -cardio -heart</t>
+  </si>
+  <si>
+    <t>S1_TC_T12</t>
+  </si>
+  <si>
+    <t>search for documents and offset value</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=5&amp;offset=2</t>
+  </si>
+  <si>
+    <t>S1_TC_T13</t>
+  </si>
+  <si>
+    <t>search for documents and restrict the number of fields returned</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=2&amp;fields=category</t>
+  </si>
+  <si>
+    <t>S1_TC_T14</t>
+  </si>
+  <si>
+    <t>Search for documents and sort on number of times cited - asc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;sort=citingsrcscount:asc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;sort=citingsrcscount:desc</t>
+  </si>
+  <si>
+    <t>Search for documents and sort on number of times cited - desc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;sort=_score:asc</t>
+  </si>
+  <si>
+    <t>Search for documents and sort on score - asc</t>
+  </si>
+  <si>
+    <t>S1_TC_T15</t>
+  </si>
+  <si>
+    <t>S1_TC_T16</t>
+  </si>
+  <si>
+    <t>S1_TC_T17</t>
+  </si>
+  <si>
+    <t>Search for documents and sort on score - desc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;sort=_score:desc</t>
+  </si>
+  <si>
+    <t>S1_TC_T18</t>
+  </si>
+  <si>
+    <t>S1_TC_T19</t>
+  </si>
+  <si>
+    <t>Search for documents and sort on pub date - des</t>
+  </si>
+  <si>
+    <t>Search for documents and sort on pub date - asc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;sort=sortdate:desc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;sort=sortdate:asc</t>
+  </si>
+  <si>
     <t/>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -521,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -729,7 +840,9 @@
       </c>
       <c r="H6"/>
       <c r="I6"/>
-      <c r="J6"/>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
       <c r="K6"/>
       <c r="L6" t="s">
         <v>23</v>
@@ -757,7 +870,9 @@
       </c>
       <c r="H7"/>
       <c r="I7"/>
-      <c r="J7"/>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
       <c r="K7"/>
       <c r="L7" t="s">
         <v>23</v>
@@ -785,9 +900,371 @@
       </c>
       <c r="H8"/>
       <c r="I8"/>
-      <c r="J8"/>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
       <c r="K8"/>
       <c r="L8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="60">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13"/>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14"/>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17"/>
+      <c r="L17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18"/>
+      <c r="L18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19"/>
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20"/>
+      <c r="L20" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified Test cases in to 1PSEARCHV3
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -52,9 +52,6 @@
     <t>STORE</t>
   </si>
   <si>
-    <t>1PSEARCH</t>
-  </si>
-  <si>
     <t>S1_TC_T1</t>
   </si>
   <si>
@@ -76,24 +73,15 @@
     <t>/details</t>
   </si>
   <si>
-    <t>?id=(S1_TC_T1_hits.hits._id)</t>
-  </si>
-  <si>
     <t>?query=bio&amp;size=1</t>
   </si>
   <si>
     <t>S1_TC_T3</t>
   </si>
   <si>
-    <t>?id=(S1_TC_T1_hits.hits._id)&amp;fields=category</t>
-  </si>
-  <si>
     <t>S1_TC_T4</t>
   </si>
   <si>
-    <t>/details/(S1_TC_T1_hits.hits._id)</t>
-  </si>
-  <si>
     <t>S1_TC_T5</t>
   </si>
   <si>
@@ -203,15 +191,6 @@
   </si>
   <si>
     <t>S1_TC_T24</t>
-  </si>
-  <si>
-    <t>/details/(S1_TC_T19_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>/details/(S1_TC_T21_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>/details/(S1_TC_T23_hits.hits._id)</t>
   </si>
   <si>
     <t>status=200&amp;&amp;{_source.title=WO||_source.fullrecord.abstract=WO||_source.keywordsplus=WO||_source.keywords=WO||_source.cuid=WO||_source.conferenceinfo=WO||_source.bibissueyear=WO||_source.address=WO||_source.addresses.suborganization=WO||_source.addresses.organization=WO||_source.identifiersxml=WO||_source.fullrecord.reprintinfo.author=WO||_source.itemxml==WO}&amp;&amp;{_source.title=FOOD||_source.fullrecord.abstract=FOOD||_source.keywordsplus=FOOD||_source.keywords=FOOD||_source.cuid=FOOD||_source.conferenceinfo=FOOD||_source.bibissueyear=FOOD||_source.address=FOOD||_source.addresses.suborganization=FOOD||_source.addresses.organization=FOOD||_source.identifiersxml=FOOD||_source.fullrecord.reprintinfo.author=FOOD||_source.itemxml==FOOD}</t>
@@ -301,6 +280,27 @@
   </si>
   <si>
     <t>Verify that for the given article id, document details are returned and validated ? rule</t>
+  </si>
+  <si>
+    <t>1PSEARCHV3</t>
+  </si>
+  <si>
+    <t>?id=wos::(S1_TC_T1_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>?id=wos::(S1_TC_T1_hits.hits._id)&amp;fields=category</t>
+  </si>
+  <si>
+    <t>/wos/details/(S1_TC_T1_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>/wos/details/(S1_TC_T19_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>/wos/details/(S1_TC_T21_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>/wos/details/(S1_TC_T23_hits.hits._id)</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
@@ -752,103 +752,103 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -857,542 +857,542 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
+        <v>82</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H20"/>
       <c r="J20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="75">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
+        <v>83</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
+        <v>84</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H22"/>
       <c r="J22" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
+        <v>87</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="H23"/>
       <c r="I23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H24"/>
       <c r="J24" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="120">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
+        <v>86</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test cases into 1PSEARCH
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
+    <sheet name="ArticalSearch" sheetId="3" r:id="rId2"/>
+    <sheet name="ProfileSearch" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="183">
   <si>
     <t>API</t>
   </si>
@@ -52,9 +54,6 @@
     <t>STORE</t>
   </si>
   <si>
-    <t>S1_TC_T1</t>
-  </si>
-  <si>
     <t>/search</t>
   </si>
   <si>
@@ -64,9 +63,6 @@
     <t>hits.hits._id</t>
   </si>
   <si>
-    <t>S1_TC_T2</t>
-  </si>
-  <si>
     <t>status=200</t>
   </si>
   <si>
@@ -76,90 +72,39 @@
     <t>?query=bio&amp;size=1</t>
   </si>
   <si>
-    <t>S1_TC_T3</t>
-  </si>
-  <si>
-    <t>S1_TC_T4</t>
-  </si>
-  <si>
-    <t>S1_TC_T5</t>
-  </si>
-  <si>
-    <t>S1_TC_T6</t>
-  </si>
-  <si>
     <t>?query=bio vascular</t>
   </si>
   <si>
     <t>?query=biotechnology&amp;size=2</t>
   </si>
   <si>
-    <t>S1_TC_T7</t>
-  </si>
-  <si>
     <t>?query=biotechnology +institute</t>
   </si>
   <si>
-    <t>S1_TC_T8</t>
-  </si>
-  <si>
     <t>?query=biotechnology +institute +cardiology</t>
   </si>
   <si>
-    <t>S1_TC_T9</t>
-  </si>
-  <si>
     <t>?query=cardi*</t>
   </si>
   <si>
-    <t>S1_TC_T10</t>
-  </si>
-  <si>
     <t>?query=biotechnology -cardio</t>
   </si>
   <si>
-    <t>S1_TC_T11</t>
-  </si>
-  <si>
     <t>?query=biotechnology -cardio -heart</t>
   </si>
   <si>
-    <t>S1_TC_T12</t>
-  </si>
-  <si>
     <t>?query=biotechnology&amp;size=5&amp;offset=2</t>
   </si>
   <si>
-    <t>S1_TC_T13</t>
-  </si>
-  <si>
     <t>?query=biotechnology&amp;size=2&amp;fields=category</t>
   </si>
   <si>
-    <t>S1_TC_T14</t>
-  </si>
-  <si>
-    <t>?query=biotechnology&amp;sort=citingsrcscount:asc</t>
-  </si>
-  <si>
     <t>?query=biotechnology&amp;sort=citingsrcscount:desc</t>
   </si>
   <si>
-    <t>S1_TC_T15</t>
-  </si>
-  <si>
-    <t>S1_TC_T16</t>
-  </si>
-  <si>
-    <t>S1_TC_T17</t>
-  </si>
-  <si>
     <t>?query=biotechnology&amp;sort=_score:desc</t>
   </si>
   <si>
-    <t>S1_TC_T18</t>
-  </si>
-  <si>
     <t>?query=biotechnology&amp;sort=sortdate:desc</t>
   </si>
   <si>
@@ -175,24 +120,6 @@
     <t>?query=food wo*&amp;size=1</t>
   </si>
   <si>
-    <t>S1_TC_T19</t>
-  </si>
-  <si>
-    <t>S1_TC_T20</t>
-  </si>
-  <si>
-    <t>S1_TC_T21</t>
-  </si>
-  <si>
-    <t>S1_TC_T22</t>
-  </si>
-  <si>
-    <t>S1_TC_T23</t>
-  </si>
-  <si>
-    <t>S1_TC_T24</t>
-  </si>
-  <si>
     <t>status=200&amp;&amp;{_source.title=WO||_source.fullrecord.abstract=WO||_source.keywordsplus=WO||_source.keywords=WO||_source.cuid=WO||_source.conferenceinfo=WO||_source.bibissueyear=WO||_source.address=WO||_source.addresses.suborganization=WO||_source.addresses.organization=WO||_source.identifiersxml=WO||_source.fullrecord.reprintinfo.author=WO||_source.itemxml==WO}&amp;&amp;{_source.title=FOOD||_source.fullrecord.abstract=FOOD||_source.keywordsplus=FOOD||_source.keywords=FOOD||_source.cuid=FOOD||_source.conferenceinfo=FOOD||_source.bibissueyear=FOOD||_source.address=FOOD||_source.addresses.suborganization=FOOD||_source.addresses.organization=FOOD||_source.identifiersxml=FOOD||_source.fullrecord.reprintinfo.author=FOOD||_source.itemxml==FOOD}</t>
   </si>
   <si>
@@ -202,12 +129,6 @@
     <t>status=200&amp;&amp;{_source.title=WOMEN||_source.fullrecord.abstract=WOMEN||_source.keywordsplus=WOMEN||_source.keywords=WOMEN||_source.cuid=WOMEN||_source.conferenceinfo=WOMEN||_source.bibissueyear=WOMEN||_source.address=WOMEN||_source.addresses.suborganization=WOMEN||_source.addresses.organization=WOMEN||_source.identifiersxml=WOMEN||_source.fullrecord.reprintinfo.author=WOMEN||_source.itemxml==WOMEN}</t>
   </si>
   <si>
-    <t>status=200&amp;&amp;_id=(S1_TC_T1_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>status=200&amp;&amp;docs._id=(S1_TC_T1_hits.hits._id)</t>
-  </si>
-  <si>
     <t>Verify that for the given article id, document details are returned</t>
   </si>
   <si>
@@ -247,13 +168,7 @@
     <t xml:space="preserve">Verify that search returned restricted matched results for the given query, category and size </t>
   </si>
   <si>
-    <t>Verify that search returned results for the given query and sort on score with desc order</t>
-  </si>
-  <si>
     <t>Verify that search returned results for the given query and sort on number of times cited with desc order</t>
-  </si>
-  <si>
-    <t>Verify that search returned results for the given query and sort on number of times cited with asc order</t>
   </si>
   <si>
     <t>Verify that search returned results for the given query and sort on publication date with desc order</t>
@@ -285,29 +200,380 @@
     <t>1PSEARCHV3</t>
   </si>
   <si>
-    <t>?id=wos::(S1_TC_T1_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>?id=wos::(S1_TC_T1_hits.hits._id)&amp;fields=category</t>
-  </si>
-  <si>
-    <t>/wos/details/(S1_TC_T1_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>/wos/details/(S1_TC_T19_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>/wos/details/(S1_TC_T21_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>/wos/details/(S1_TC_T23_hits.hits._id)</t>
+    <t>OPQA-375</t>
+  </si>
+  <si>
+    <t>OPQA-726</t>
+  </si>
+  <si>
+    <t>OPQA-375_1</t>
+  </si>
+  <si>
+    <t>OPQA-727</t>
+  </si>
+  <si>
+    <t>OPQA-728</t>
+  </si>
+  <si>
+    <t>OPQA-729</t>
+  </si>
+  <si>
+    <t>OPQA-729_1</t>
+  </si>
+  <si>
+    <t>OPQA-249</t>
+  </si>
+  <si>
+    <t>OPQA-730</t>
+  </si>
+  <si>
+    <t>OPQA-730_1</t>
+  </si>
+  <si>
+    <t>OPQA-731</t>
+  </si>
+  <si>
+    <t>OPQA-732</t>
+  </si>
+  <si>
+    <t>OPQA-283</t>
+  </si>
+  <si>
+    <t>OPQA-733</t>
+  </si>
+  <si>
+    <t>OPQA-287</t>
+  </si>
+  <si>
+    <t>OPQA-301</t>
+  </si>
+  <si>
+    <t>OPQA-734</t>
+  </si>
+  <si>
+    <t>OPQA-375_2</t>
+  </si>
+  <si>
+    <t>OPQA-254</t>
+  </si>
+  <si>
+    <t>OPQA-254_1</t>
+  </si>
+  <si>
+    <t>OPQA-252</t>
+  </si>
+  <si>
+    <t>OPQA-252_1</t>
+  </si>
+  <si>
+    <t>OPQA-358</t>
+  </si>
+  <si>
+    <t>Verify that search returned results for the given query and sort on score(Relevance) with desc order</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-358_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>?id=wos::(OPQA-358_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>status=200&amp;&amp;docs._id=(OPQA-358_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>?id=wos::(OPQA-358_hits.hits._id)&amp;fields=category</t>
+  </si>
+  <si>
+    <t>status=200&amp;&amp;_id=(OPQA-358_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-734_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-254_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-252_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>OPQA-896</t>
+  </si>
+  <si>
+    <t>Verify that to get articles for query</t>
+  </si>
+  <si>
+    <t>/wos/search</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=1&amp;fields=citingsrcslocalcount&amp;sort=citingsrcslocalcount:desc</t>
+  </si>
+  <si>
+    <t>hits.hits._id||hits.hits.fields.citingsrcslocalcount</t>
+  </si>
+  <si>
+    <t>Verify that to get full article  data for given id</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-896_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>status=200||_source.citingsrcslocalcount=(OPQA-896_hits.hits.fields.citingsrcslocalcount)</t>
+  </si>
+  <si>
+    <t>OPQA-344</t>
+  </si>
+  <si>
+    <t>Verify that get comments count for the article works as expected</t>
+  </si>
+  <si>
+    <t>1PAUTHORING</t>
+  </si>
+  <si>
+    <t>/comments/count/(OPQA-896_hits.hits._id)/wos</t>
+  </si>
+  <si>
+    <t>counterValue</t>
+  </si>
+  <si>
+    <t>OPQA-345</t>
+  </si>
+  <si>
+    <t>Verify that get comment statistics for the article and validate comment count</t>
+  </si>
+  <si>
+    <t>/statistics/wos</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-896_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>OPQA-896||OPQA-344</t>
+  </si>
+  <si>
+    <t>status=200||commentCount=(OPQA-344_counterValue)</t>
+  </si>
+  <si>
+    <t>OPQA-896_1</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=4</t>
+  </si>
+  <si>
+    <t>hits.hits._id[0]||hits.hits._id[1]||hits.hits._id[2]||hits.hits._id[3]</t>
+  </si>
+  <si>
+    <t>Verify that to get multiple articles data by passing multiple id's</t>
+  </si>
+  <si>
+    <t>/wos/details</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-896_1_hits.hits._id[0])&amp;id=(OPQA-896_1_hits.hits._id[1])&amp;id=(OPQA-896_1_hits.hits._id[2])&amp;id=(OPQA-896_1_hits.hits._id[3])</t>
+  </si>
+  <si>
+    <t>status=200||docs._id[0]=(OPQA-896_1_hits.hits._id[0])||docs._id[1]=(OPQA-896_1_hits.hits._id[1])||docs._id[2]=(OPQA-896_1_hits.hits._id[2])||docs._id[3]=(OPQA-896_1_hits.hits._id[3])</t>
+  </si>
+  <si>
+    <t>Verify that to sort articles with times cited count</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=100&amp;fields=citingsrcslocalcount&amp;sort=citingsrcslocalcount:desc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=100&amp;fields=score&amp;sort=_score:desc</t>
+  </si>
+  <si>
+    <t>Verify that to sort articles with pub date desc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=100&amp;fields=sortdate&amp;sort=sortdate:desc</t>
+  </si>
+  <si>
+    <t>Verify that to sort articles with pub date asc</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=100&amp;fields=sortdate&amp;sort=sortdate:asc</t>
+  </si>
+  <si>
+    <t>OPQA-909</t>
+  </si>
+  <si>
+    <t>OPQA-910</t>
+  </si>
+  <si>
+    <t>Verify that to sort articles with Relevance</t>
+  </si>
+  <si>
+    <t>OPQA-911</t>
+  </si>
+  <si>
+    <t>OPQA-911_1</t>
+  </si>
+  <si>
+    <t>OPQA-911_2</t>
+  </si>
+  <si>
+    <t>OPQA-911_3</t>
+  </si>
+  <si>
+    <t>/people/search</t>
+  </si>
+  <si>
+    <t>OPQA-434</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles</t>
+  </si>
+  <si>
+    <t>OPQA-435</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get Profile details by passing profile id</t>
+  </si>
+  <si>
+    <t>/people/details/(OPQA-434_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>?query=Project&amp;size=1&amp;fields=fullrecord.summary.contenttype</t>
+  </si>
+  <si>
+    <t>status=200||_type=people||_id=(OPQA-434_hits.hits._id)||_source.authors=Project</t>
+  </si>
+  <si>
+    <t>OPQA-436</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles with first name</t>
+  </si>
+  <si>
+    <t>?query=Project&amp;size=1</t>
+  </si>
+  <si>
+    <t>OPQA-501</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get profile and verify the firstname</t>
+  </si>
+  <si>
+    <t>1PPROFILE</t>
+  </si>
+  <si>
+    <t>/users/user/(OPQA-436_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project</t>
+  </si>
+  <si>
+    <t>OPQA-437</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles with Last name</t>
+  </si>
+  <si>
+    <t>?query=Neon1&amp;size=1</t>
+  </si>
+  <si>
+    <t>OPQA-501_1</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get profile and verify the lastname</t>
+  </si>
+  <si>
+    <t>/users/user/(OPQA-437_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>status=200||lastName=Neon1</t>
+  </si>
+  <si>
+    <t>OPQA-438</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles with intrests</t>
+  </si>
+  <si>
+    <t>?query="API AUTOMATION"&amp;size=1</t>
+  </si>
+  <si>
+    <t>OPQA-501_2</t>
+  </si>
+  <si>
+    <t>/users/user/(OPQA-438_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>status=200||interest=API AUTOMATION</t>
+  </si>
+  <si>
+    <t>OPQA-439</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles with Title/Role</t>
+  </si>
+  <si>
+    <t>?query="Project Neon1"&amp;fields=authors</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.authors=Project Neon1</t>
+  </si>
+  <si>
+    <t>OPQA-439_1</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles with Role</t>
+  </si>
+  <si>
+    <t>?query=QA&amp;fields=role</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.role=QA</t>
+  </si>
+  <si>
+    <t>OPQA-440</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles with Country</t>
+  </si>
+  <si>
+    <t>?query=india&amp;fields=country</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.country=india</t>
+  </si>
+  <si>
+    <t>OPQA-441</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles with Primary Institution</t>
+  </si>
+  <si>
+    <t>?query=TR&amp;size=1&amp;agg=institution</t>
+  </si>
+  <si>
+    <t>status=200||aggregations.institution_filter.institution.buckets.key=TR</t>
+  </si>
+  <si>
+    <t>OPQA-442</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles which match the query with wild character and should not contain multiple words</t>
+  </si>
+  <si>
+    <t>?query=Proj* -Neon2</t>
+  </si>
+  <si>
+    <t>OPQA-443</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles and restrict the number of fields returned</t>
+  </si>
+  <si>
+    <t>?query=Project&amp;size=2&amp;fields=category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +595,20 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -376,7 +656,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -393,6 +673,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -690,15 +984,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
-      <selection activeCell="L25" sqref="L2:L25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="98.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="44" bestFit="1" customWidth="1" collapsed="1"/>
@@ -738,7 +1032,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
@@ -752,103 +1046,103 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -857,546 +1151,1285 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19"/>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="75">
+      <c r="A20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21"/>
+      <c r="J21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30">
+      <c r="A23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23"/>
+      <c r="J23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="120">
+      <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20"/>
-      <c r="J20" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="75">
-      <c r="A21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21"/>
-      <c r="I21" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30">
-      <c r="A22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22"/>
-      <c r="J22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="60">
-      <c r="A23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23"/>
-      <c r="I23" t="s">
-        <v>55</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="30">
-      <c r="A24" s="1" t="s">
+      <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="G24" t="s">
-        <v>52</v>
-      </c>
       <c r="H24"/>
-      <c r="J24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="120">
-      <c r="A25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" t="s">
-        <v>1</v>
-      </c>
-      <c r="H25"/>
-      <c r="I25" t="s">
-        <v>57</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>59</v>
+      <c r="I24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="78.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="57" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.85546875" style="6" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="A2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30">
+      <c r="A3" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3"/>
+      <c r="I3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="1:12" ht="30">
+      <c r="A4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="8"/>
+      <c r="I4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" ht="45">
+      <c r="A6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75">
+      <c r="A7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7"/>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="A6" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="I7" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="I3" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I4" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I5" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="A3" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-909"/>
+    <hyperlink ref="A7" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-910"/>
+    <hyperlink ref="A8" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-911"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="44.7109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="47" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="A2" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="31.5">
+      <c r="A3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3"/>
+      <c r="I3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="31.5">
+      <c r="A4" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="31.5">
+      <c r="A5" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="31.5">
+      <c r="A6" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="31.5">
+      <c r="A7" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="31.5">
+      <c r="A8" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>157</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="31.5">
+      <c r="A9" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="31.5">
+      <c r="A10" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>163</v>
+      </c>
+      <c r="J10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75">
+      <c r="A11" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>167</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="31.5">
+      <c r="A12" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>171</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="31.5">
+      <c r="A13" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="47.25">
+      <c r="A14" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>179</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="31.5">
+      <c r="A15" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>182</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding test cases to post search. Removing testcases in profile search
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="ArticalSearch" sheetId="3" r:id="rId2"/>
     <sheet name="ProfileSearch" sheetId="4" r:id="rId3"/>
+    <sheet name="PostSearch" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="221">
   <si>
     <t>API</t>
   </si>
@@ -576,6 +577,111 @@
   </si>
   <si>
     <t>OPQA-920_1</t>
+  </si>
+  <si>
+    <t>OPQA-1158</t>
+  </si>
+  <si>
+    <t>Verify that to get total posts count for query</t>
+  </si>
+  <si>
+    <t>?query=Post&amp;aggregateOnly=true&amp;agg=contenttypenavigator</t>
+  </si>
+  <si>
+    <t>status=200||aggregations.contenttypenavigator_filter.contenttypenavigator.buckets.key=Posts</t>
+  </si>
+  <si>
+    <t>OPQA-897</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for posts</t>
+  </si>
+  <si>
+    <t>/posts/search</t>
+  </si>
+  <si>
+    <t>?query=Post&amp;size=1</t>
+  </si>
+  <si>
+    <t>status=200&amp;&amp;{hits.hits._source.firstName=Project||hits.hits._type=posts}</t>
+  </si>
+  <si>
+    <t>OPQA-1159</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get Post details by id</t>
+  </si>
+  <si>
+    <t>/posts/details/(OPQA-897_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>status=200||_type=posts||_id=(OPQA-897_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>Verify that get comments count for the post</t>
+  </si>
+  <si>
+    <t>/comments/count/(OPQA-897_hits.hits._id)/posts</t>
+  </si>
+  <si>
+    <t>Verify that get comment statistics for the post and validate comment count</t>
+  </si>
+  <si>
+    <t>/statistics/posts</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-897_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>OPQA-897||OPQA-344</t>
+  </si>
+  <si>
+    <t>OPQA-897_1</t>
+  </si>
+  <si>
+    <t>?query=Post&amp;size=4</t>
+  </si>
+  <si>
+    <t>OPQA-1159_1</t>
+  </si>
+  <si>
+    <t>Verify that to get multiple posts data by passing multiple id's</t>
+  </si>
+  <si>
+    <t>/posts/details</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-897_1_hits.hits._id[0])&amp;id=(OPQA-897_1_hits.hits._id[1])&amp;id=(OPQA-897_1_hits.hits._id[2])&amp;id=(OPQA-897_1_hits.hits._id[3])</t>
+  </si>
+  <si>
+    <t>status=200||docs._id[0]=(OPQA-897_1_hits.hits._id[0])||docs._id[1]=(OPQA-897_1_hits.hits._id[1])||docs._id[2]=(OPQA-897_1_hits.hits._id[2])||docs._id[3]=(OPQA-897_1_hits.hits._id[3])</t>
+  </si>
+  <si>
+    <t>OPQA-1126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that to sort posts with relevance </t>
+  </si>
+  <si>
+    <t>?query=Post&amp;fields=score&amp;sort=_score:desc</t>
+  </si>
+  <si>
+    <t>OPQA-1126_1</t>
+  </si>
+  <si>
+    <t>Verify that to sort posts with pub date desc</t>
+  </si>
+  <si>
+    <t>?query=Post&amp;fields=sortdate&amp;sort=sortdate:desc</t>
+  </si>
+  <si>
+    <t>OPQA-1126_2</t>
+  </si>
+  <si>
+    <t>Verify that to sort posts with pub date asc</t>
+  </si>
+  <si>
+    <t>?query=Post&amp;fields=sortdate&amp;sort=sortdate:asc</t>
   </si>
 </sst>
 </file>
@@ -665,7 +771,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -697,6 +803,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2026,7 +2135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L17"/>
     </sheetView>
   </sheetViews>
@@ -2458,7 +2567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
         <v>185</v>
       </c>
@@ -2484,7 +2593,6 @@
         <v>15</v>
       </c>
       <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2495,4 +2603,348 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="53" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="72.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="145.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="31.5">
+      <c r="A2" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1"/>
+      <c r="J2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="31.5">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="31.5">
+      <c r="A4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="8"/>
+      <c r="I5" t="s">
+        <v>190</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30">
+      <c r="A6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" t="s">
+        <v>204</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" ht="45">
+      <c r="A7" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="1"/>
+      <c r="J7" t="s">
+        <v>194</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>205</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="H10"/>
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I6" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I8" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="A2" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1158"/>
+    <hyperlink ref="A3" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-897"/>
+    <hyperlink ref="A4" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1159"/>
+    <hyperlink ref="A8" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1159"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test cases for patent search
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="ArticalSearch" sheetId="3" r:id="rId2"/>
-    <sheet name="ProfileSearch" sheetId="4" r:id="rId3"/>
-    <sheet name="PostSearch" sheetId="5" r:id="rId4"/>
+    <sheet name="PatentSearch" sheetId="6" r:id="rId3"/>
+    <sheet name="ProfileSearch" sheetId="4" r:id="rId4"/>
+    <sheet name="PostSearch" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="247">
   <si>
     <t>API</t>
   </si>
@@ -682,6 +683,84 @@
   </si>
   <si>
     <t>?query=Post&amp;fields=sortdate&amp;sort=sortdate:asc</t>
+  </si>
+  <si>
+    <t>Verify that to get total patents count for query</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;aggregateOnly=true&amp;agg=contenttypenavigator</t>
+  </si>
+  <si>
+    <t>status=200||aggregations.contenttypenavigator_filter.contenttypenavigator.buckets.key=Patents</t>
+  </si>
+  <si>
+    <t>OPQA-898</t>
+  </si>
+  <si>
+    <t>Verify that to get patents for query</t>
+  </si>
+  <si>
+    <t>/patents/search</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=1</t>
+  </si>
+  <si>
+    <t>Verify that to get full patent  data for given patent number</t>
+  </si>
+  <si>
+    <t>/patents/details/(OPQA-898_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>Verify that get comments count for the patent</t>
+  </si>
+  <si>
+    <t>Verify that get comment statistics for the patent and validate comment count</t>
+  </si>
+  <si>
+    <t>OPQA-898_1</t>
+  </si>
+  <si>
+    <t>Verify that to get multiple patents data by passing multiple id's</t>
+  </si>
+  <si>
+    <t>/patents/details</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-898_1_hits.hits._id[0])&amp;id=(OPQA-898_1_hits.hits._id[1])&amp;id=(OPQA-898_1_hits.hits._id[2])&amp;id=(OPQA-898_1_hits.hits._id[3])</t>
+  </si>
+  <si>
+    <t>status=200||docs._id[0]=(OPQA-898_1_hits.hits._id[0])||docs._id[1]=(OPQA-898_1_hits.hits._id[1])||docs._id[2]=(OPQA-898_1_hits.hits._id[2])||docs._id[3]=(OPQA-898_1_hits.hits._id[3])</t>
+  </si>
+  <si>
+    <t>Verify that to sort patents with times cited count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that to sort patents with relevance </t>
+  </si>
+  <si>
+    <t>Verify that to sort patents with pub date desc</t>
+  </si>
+  <si>
+    <t>Verify that to sort patents with pub date asc</t>
+  </si>
+  <si>
+    <t>OPQA-1176</t>
+  </si>
+  <si>
+    <t>OPQA-1176_1</t>
+  </si>
+  <si>
+    <t>OPQA-1177</t>
+  </si>
+  <si>
+    <t>OPQA-1177_1</t>
+  </si>
+  <si>
+    <t>OPQA-1177_2</t>
+  </si>
+  <si>
+    <t>OPQA-1177_3</t>
   </si>
 </sst>
 </file>
@@ -2133,6 +2212,447 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="66.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="145.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="31.5">
+      <c r="A2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1"/>
+      <c r="J2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30">
+      <c r="A4" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4"/>
+      <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="8"/>
+      <c r="I5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45">
+      <c r="A6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" ht="45">
+      <c r="A7" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>232</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12"/>
+      <c r="J12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75">
+      <c r="A13" s="8"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="1"/>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75">
+      <c r="A14" s="8"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="1"/>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
+      <c r="A15" s="8"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="1"/>
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
+      <c r="A16" s="8"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="1"/>
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75">
+      <c r="A17" s="8"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="1"/>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75">
+      <c r="A18" s="8"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="1"/>
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75">
+      <c r="A19" s="8"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="H19"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.75">
+      <c r="A20" s="8"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="8"/>
+      <c r="H20"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75">
+      <c r="A21" s="8"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="8"/>
+      <c r="F21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75">
+      <c r="A22" s="8"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="8"/>
+      <c r="H22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-898"/>
+    <hyperlink ref="A2" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1158"/>
+    <hyperlink ref="A7" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="I8" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="I5" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I6" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-910"/>
+    <hyperlink ref="A4" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1176"/>
+    <hyperlink ref="A9" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1177"/>
+    <hyperlink ref="A10" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1177"/>
+    <hyperlink ref="A11:A12" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1177"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2605,7 +3125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding Test cases to Notify Adding test cases Search Reducing time delay for notify test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="271">
   <si>
     <t>API</t>
   </si>
@@ -761,6 +761,78 @@
   </si>
   <si>
     <t>OPQA-1177_3</t>
+  </si>
+  <si>
+    <t>OPQA-898_2</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=1&amp;fields=title,patentno,sortdate,abstract,authors</t>
+  </si>
+  <si>
+    <t>OPQA-1225</t>
+  </si>
+  <si>
+    <t>Verify that to search patents by passing title</t>
+  </si>
+  <si>
+    <t>?query="(OPQA-898_2_hits.hits.fields.title)"&amp;fields=title</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.title=(OPQA-898_2_hits.hits.fields.title)</t>
+  </si>
+  <si>
+    <t>OPQA-1225_1</t>
+  </si>
+  <si>
+    <t>Verify that to search patents by passing patent number</t>
+  </si>
+  <si>
+    <t>?query=(OPQA-898_2_hits.hits.fields.patentno)&amp;fields=patentno</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.patentno=(OPQA-898_2_hits.hits.fields.patentno)</t>
+  </si>
+  <si>
+    <t>OPQA-898_3</t>
+  </si>
+  <si>
+    <t>?query=EP1890144B1&amp;size=1&amp;fields=abstract</t>
+  </si>
+  <si>
+    <t>hits.hits.fields.abstract</t>
+  </si>
+  <si>
+    <t>OPQA-1225_2</t>
+  </si>
+  <si>
+    <t>Verify that to search patents by passing abstract</t>
+  </si>
+  <si>
+    <t>?query=%22(OPQA-898_3_hits.hits.fields.abstract)%22&amp;fields=abstract</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.abstract=(OPQA-898_3_hits.hits.fields.abstract)</t>
+  </si>
+  <si>
+    <t>OPQA-1225_3</t>
+  </si>
+  <si>
+    <t>?query="Lakshminath, Anand"&amp;fields=authors</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.authors=Lakshminath</t>
+  </si>
+  <si>
+    <t>OPQA-1225_4</t>
+  </si>
+  <si>
+    <t>?query="Lakshminath, Anand"&amp;fields=assignee</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.assignee=Lakshminath</t>
+  </si>
+  <si>
+    <t>hits.hits.fields.title||hits.hits.fields.patentno</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L11"/>
     </sheetView>
   </sheetViews>
@@ -2195,18 +2267,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="A6" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
-    <hyperlink ref="I7" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
-    <hyperlink ref="I3" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="I4" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="I5" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="A3" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-909"/>
-    <hyperlink ref="A7" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-910"/>
-    <hyperlink ref="A8" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-911"/>
+    <hyperlink ref="I7" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="I3" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I4" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I5" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2214,8 +2281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L12"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2565,51 +2632,194 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="8"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="1"/>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75">
-      <c r="A14" s="8"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="1"/>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>251</v>
+      </c>
       <c r="H14"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75">
-      <c r="A15" s="8"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="1"/>
+      <c r="I14" t="s">
+        <v>247</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="H15"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="8"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="1"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75">
-      <c r="A17" s="8"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="1"/>
+      <c r="I15" t="s">
+        <v>247</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30">
+      <c r="A17" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>262</v>
+      </c>
       <c r="H17"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75">
-      <c r="A18" s="8"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="1"/>
+      <c r="I17" t="s">
+        <v>257</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30">
+      <c r="A18" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="H18"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75">
-      <c r="A19" s="8"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
+      <c r="J18" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30">
+      <c r="A19" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>268</v>
+      </c>
       <c r="H19"/>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75">
+      <c r="J19" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75">
       <c r="A20" s="8"/>
       <c r="B20" s="13"/>
       <c r="C20" s="9"/>
@@ -2617,7 +2827,7 @@
       <c r="H20"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75">
+    <row r="21" spans="1:10" ht="15.75">
       <c r="A21" s="8"/>
       <c r="B21" s="13"/>
       <c r="C21" s="9"/>
@@ -2626,7 +2836,7 @@
       <c r="H21" s="11"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75">
+    <row r="22" spans="1:10" ht="15.75">
       <c r="A22" s="8"/>
       <c r="B22" s="13"/>
       <c r="C22" s="9"/>
@@ -2635,17 +2845,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-898"/>
-    <hyperlink ref="A2" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1158"/>
-    <hyperlink ref="A7" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
-    <hyperlink ref="I8" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
-    <hyperlink ref="I5" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="I6" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="A8" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-910"/>
-    <hyperlink ref="A4" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1176"/>
-    <hyperlink ref="A9" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1177"/>
-    <hyperlink ref="A10" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1177"/>
-    <hyperlink ref="A11:A12" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1177"/>
+    <hyperlink ref="I8" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="I5" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I6" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3115,13 +3317,8 @@
       <c r="K17" s="8"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
-    <hyperlink ref="A16" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-920"/>
-    <hyperlink ref="A17" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-920"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3460,10 +3657,6 @@
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
     <hyperlink ref="I8" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
-    <hyperlink ref="A2" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1158"/>
-    <hyperlink ref="A3" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-897"/>
-    <hyperlink ref="A4" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1159"/>
-    <hyperlink ref="A8" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1159"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Test cases into article search
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="312">
   <si>
     <t>API</t>
   </si>
@@ -833,6 +833,129 @@
   </si>
   <si>
     <t>hits.hits.fields.title||hits.hits.fields.patentno</t>
+  </si>
+  <si>
+    <t>OPQA-896_2</t>
+  </si>
+  <si>
+    <t>Verify that to search articles for query</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=1&amp;fields=title,source,sortdate,abstract&amp;sort=citingsrcslocalcount:desc</t>
+  </si>
+  <si>
+    <t>hits.hits._id||hits.hits.fields.title||hits.hits.fields.abstract||hits.hits.fields.source</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>OPQA-1315</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing title</t>
+  </si>
+  <si>
+    <t>?query="(OPQA-896_2_hits.hits.fields.title)"&amp;fields=title</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.title=(OPQA-896_2_hits.hits.fields.title)</t>
+  </si>
+  <si>
+    <t>OPQA-1315_1</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing abstract</t>
+  </si>
+  <si>
+    <t>?query="(OPQA-896_2_hits.hits.fields.abstract)"&amp;fields=abstract</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.abstract=(OPQA-896_2_hits.hits.fields.abstract)</t>
+  </si>
+  <si>
+    <t>OPQA-1315_2</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing publication name</t>
+  </si>
+  <si>
+    <t>?query="(OPQA-896_2_hits.hits.fields.source)"&amp;fields=source&amp;sort=citingsrcslocalcount:desc</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.source=(OPQA-896_2_hits.hits.fields.source)</t>
+  </si>
+  <si>
+    <t>OPQA-1315_3</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing authors name</t>
+  </si>
+  <si>
+    <t>?query="LAEMMLI, UK"&amp;fields=fullrecord.summary.authors</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields."fullrecord.summary.authors"=LAEMMLI, UK</t>
+  </si>
+  <si>
+    <t>OPQA-1315_4</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing publication year</t>
+  </si>
+  <si>
+    <t>?query="1970"&amp;fields=fullrecord.summary.pubdate&amp;sort=citingsrcslocalcount:desc</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields."fullrecord.summary.pubdate"=1970</t>
+  </si>
+  <si>
+    <t>OPQA-1315_5</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing issn number</t>
+  </si>
+  <si>
+    <t>?query="0028-0836"&amp;fields=fullrecord.issn&amp;sort=citingsrcslocalcount:desc</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields."fullrecord.issn"=0028-0836</t>
+  </si>
+  <si>
+    <t>OPQA-1315_6</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing Keywordplus</t>
+  </si>
+  <si>
+    <t>?query="ANTIBIOTIC-ASSOCIATED DIARRHEA" "UPPER GASTROINTESTINAL-TRACT" " POLYMERASE-CHAIN-REACTION"&amp;fields=keywordsplus</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.keywordsplus=ANTIBIOTIC-ASSOCIATED DIARRHEA</t>
+  </si>
+  <si>
+    <t>OPQA-1315_7</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing Keywords</t>
+  </si>
+  <si>
+    <t>?query="Bio-K"  "Lactobacillus"  "probiotic"  "Clostridium difficile"  "prevention"&amp;fields=keywords</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.keywords=Bio-K||hits.hits.fields.keywords=Lactobacillus||hits.hits.fields.keywords=probiotic</t>
+  </si>
+  <si>
+    <t>OPQA-1315_8</t>
+  </si>
+  <si>
+    <t>Verify that to search articles by passing funding agency</t>
+  </si>
+  <si>
+    <t>?query="BIO K PLUS INTERNATIONAL"&amp;fields=fundingag</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.fundingag=BIO K PLUS INTERNATIONAL</t>
   </si>
 </sst>
 </file>
@@ -1939,15 +2062,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="59.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -2264,6 +2387,288 @@
         <v>15</v>
       </c>
       <c r="K11"/>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L12" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30">
+      <c r="A16" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30">
+      <c r="A17" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30">
+      <c r="A18" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="45">
+      <c r="A19" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45">
+      <c r="A20" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30">
+      <c r="A21" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" t="s">
+        <v>275</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3326,7 +3731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added test cases into Posts Search
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="347">
   <si>
     <t>API</t>
   </si>
@@ -956,6 +956,111 @@
   </si>
   <si>
     <t>status=200||hits.hits.fields.fundingag=BIO K PLUS INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>OPQA-360</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a post and publish it.</t>
+  </si>
+  <si>
+    <t>/posts/</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>{"title":"Creating Post For API Search Testing","content":"This post is creating for search testing"}</t>
+  </si>
+  <si>
+    <t>Verify that to search posts by passing title</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||found=true</t>
+  </si>
+  <si>
+    <t>id||title||content</t>
+  </si>
+  <si>
+    <t>OPQA-494</t>
+  </si>
+  <si>
+    <t>Verify that get user profile information</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>firstName||lastName||primaryInstitution</t>
+  </si>
+  <si>
+    <t>OPQA-1317</t>
+  </si>
+  <si>
+    <t>?query="(OPQA-360_title)"&amp;fields=sortdate,title&amp;sort=sortdate:desc&amp;size=1</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.title=(OPQA-360_title)</t>
+  </si>
+  <si>
+    <t>OPQA-1317_1</t>
+  </si>
+  <si>
+    <t>Verify that to search posts by passing content</t>
+  </si>
+  <si>
+    <t>?query="(OPQA-360_content)"&amp;fields=sortdate,posttext&amp;sort=sortdate:desc&amp;size=1</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.posttext=(OPQA-360_content)</t>
+  </si>
+  <si>
+    <t>OPQA-1317_2</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for posts by passing author's Institution</t>
+  </si>
+  <si>
+    <t>?query="(OPQA-494_primaryInstitution)"&amp;fields=title,authors&amp;sort=sortdate:desc&amp;size=1</t>
+  </si>
+  <si>
+    <t>OPQA-494||OPQA-360</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits.fields.title=(OPQA-360_title)||hits.hits.fields.authors=(OPQA-494_firstName) (OPQA-494_lastName)</t>
+  </si>
+  <si>
+    <t>OPQA-1317_3</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for posts by passing author's name</t>
+  </si>
+  <si>
+    <t>?query="(OPQA-494_firstName) (OPQA-494_lastName)"&amp;fields=title,authors&amp;sort=sortdate:desc&amp;size=1</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits._id=(OPQA-360_id)||hits.hits.fields.authors=(OPQA-494_firstName) (OPQA-494_lastName)</t>
+  </si>
+  <si>
+    <t>OPQA-1076</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to delete their post</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||id=(OPQA-360_id)</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1150,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1080,6 +1185,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2064,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2388,7 +2496,7 @@
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:12" ht="30">
+    <row r="12" spans="1:12" ht="60">
       <c r="A12" s="5" t="s">
         <v>271</v>
       </c>
@@ -2474,7 +2582,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45">
+    <row r="15" spans="1:12" ht="30">
       <c r="A15" s="5" t="s">
         <v>284</v>
       </c>
@@ -2558,7 +2666,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="30">
+    <row r="18" spans="1:12">
       <c r="A18" s="5" t="s">
         <v>296</v>
       </c>
@@ -2586,7 +2694,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="45">
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="5" t="s">
         <v>300</v>
       </c>
@@ -3729,22 +3837,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="53" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="52.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="72.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="38.140625" style="6" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="145.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="24.7109375" customWidth="1" collapsed="1"/>
@@ -3789,7 +3897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="31.5">
+    <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>186</v>
       </c>
@@ -3816,7 +3924,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="31.5">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -3845,7 +3953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="31.5">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" t="s">
         <v>195</v>
       </c>
@@ -3861,7 +3969,6 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="H4"/>
       <c r="I4" t="s">
         <v>190</v>
       </c>
@@ -3869,7 +3976,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30">
+    <row r="5" spans="1:12">
       <c r="A5" s="5" t="s">
         <v>94</v>
       </c>
@@ -3887,7 +3994,7 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="8"/>
+      <c r="H5" s="10"/>
       <c r="I5" t="s">
         <v>190</v>
       </c>
@@ -3918,7 +4025,7 @@
       <c r="G6" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="10"/>
       <c r="I6" t="s">
         <v>204</v>
       </c>
@@ -3975,7 +4082,6 @@
       <c r="G8" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="H8"/>
       <c r="I8" t="s">
         <v>205</v>
       </c>
@@ -3983,7 +4089,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30">
+    <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
         <v>212</v>
       </c>
@@ -4003,14 +4109,14 @@
       <c r="G9" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="30">
+    <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
         <v>215</v>
       </c>
@@ -4029,12 +4135,11 @@
       <c r="G10" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="H10"/>
       <c r="J10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30">
+    <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
         <v>218</v>
       </c>
@@ -4053,10 +4158,202 @@
       <c r="G11" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H11"/>
       <c r="J11" s="1" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="12" spans="1:12" ht="45">
+      <c r="A12" t="s">
+        <v>312</v>
+      </c>
+      <c r="B12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E12" t="s">
+        <v>315</v>
+      </c>
+      <c r="F12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="J12" t="s">
+        <v>319</v>
+      </c>
+      <c r="K12" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14" t="s">
+        <v>312</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="H15"/>
+      <c r="I15" t="s">
+        <v>312</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="31.5">
+      <c r="A16" t="s">
+        <v>332</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>334</v>
+      </c>
+      <c r="H16"/>
+      <c r="I16" t="s">
+        <v>335</v>
+      </c>
+      <c r="J16" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="31.5">
+      <c r="A17" t="s">
+        <v>337</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>339</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17" t="s">
+        <v>335</v>
+      </c>
+      <c r="J17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>341</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="K18" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Modified 1PSEARCH test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -3839,8 +3839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3897,231 +3897,233 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:12" ht="45">
+      <c r="A2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="J2" t="s">
+        <v>319</v>
+      </c>
+      <c r="K2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75">
+      <c r="A3" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B3" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="1"/>
-      <c r="J2" t="s">
-        <v>189</v>
-      </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>194</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="15.75">
       <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="1"/>
+      <c r="J4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75">
+      <c r="A5" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B5" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>190</v>
-      </c>
-      <c r="J4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
       <c r="I5" t="s">
         <v>190</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30">
+      <c r="J5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="10" t="s">
-        <v>203</v>
-      </c>
+      <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" t="s">
         <v>204</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" ht="45">
-      <c r="A7" s="8" t="s">
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B8" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="1"/>
-      <c r="J7" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="1"/>
+      <c r="J8" t="s">
         <v>194</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45">
-      <c r="A8" t="s">
+    <row r="9" spans="1:12" ht="45">
+      <c r="A9" t="s">
         <v>207</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>205</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>54</v>
@@ -4132,19 +4134,23 @@
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>217</v>
-      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>54</v>
@@ -4156,39 +4162,33 @@
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="45">
-      <c r="A12" t="s">
-        <v>312</v>
-      </c>
-      <c r="B12" t="s">
-        <v>313</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E12" t="s">
-        <v>315</v>
-      </c>
-      <c r="F12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="J12" t="s">
-        <v>319</v>
-      </c>
-      <c r="K12" t="s">
-        <v>320</v>
+      <c r="J12" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
@@ -4357,8 +4357,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I6" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="I8" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="I7" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I9" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed failing test cases in to search
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -1484,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1544,70 +1544,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>54</v>
+    <row r="2" spans="1:12" ht="45">
+      <c r="A2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>314</v>
+      </c>
+      <c r="E2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="J2" t="s">
+        <v>319</v>
+      </c>
+      <c r="K2" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>54</v>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
@@ -1633,64 +1633,66 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
         <v>77</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="5" t="s">
-        <v>15</v>
+      <c r="I6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>54</v>
@@ -1703,7 +1705,7 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1712,12 +1714,12 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="30">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>54</v>
@@ -1730,7 +1732,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1741,10 +1743,10 @@
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>54</v>
@@ -1757,7 +1759,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1766,12 +1768,12 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" ht="30">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>54</v>
@@ -1784,7 +1786,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1793,12 +1795,12 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="30">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>54</v>
@@ -1811,7 +1813,7 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1822,10 +1824,10 @@
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>54</v>
@@ -1838,7 +1840,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1847,12 +1849,12 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" ht="30">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -1865,7 +1867,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1876,10 +1878,10 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -1892,7 +1894,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1901,12 +1903,12 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="30">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
@@ -1918,22 +1920,22 @@
         <v>1</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="5" t="s">
-        <v>174</v>
+      <c r="G15" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" ht="30">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>183</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -1945,8 +1947,8 @@
         <v>1</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
-        <v>27</v>
+      <c r="G16" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1955,12 +1957,12 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="30">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>54</v>
@@ -1972,8 +1974,8 @@
         <v>1</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="6" t="s">
-        <v>176</v>
+      <c r="G17" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1982,12 +1984,12 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="30">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>54</v>
@@ -2000,7 +2002,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2011,10 +2013,10 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
+        <v>70</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
@@ -2022,143 +2024,170 @@
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="E19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>28</v>
       </c>
-      <c r="H19"/>
-      <c r="J19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="H20"/>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="75">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:11" ht="75">
+      <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20"/>
-      <c r="I20" t="s">
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:11" ht="30">
+      <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>29</v>
       </c>
-      <c r="H21"/>
-      <c r="J21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="H22"/>
+      <c r="J22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="60">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:11" ht="60">
+      <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22"/>
-      <c r="I22" t="s">
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23" t="s">
         <v>73</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J23" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="30">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E23" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
         <v>30</v>
       </c>
-      <c r="H23"/>
-      <c r="J23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="H24"/>
+      <c r="J24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="120">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:11" ht="120">
+      <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24"/>
-      <c r="I24" t="s">
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25"/>
+      <c r="I25" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J25" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3837,10 +3866,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3897,233 +3926,231 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45">
-      <c r="A2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" t="s">
-        <v>96</v>
+    <row r="2" spans="1:12" ht="15.75">
+      <c r="A2" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F2" t="s">
-        <v>316</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>317</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>319</v>
-      </c>
-      <c r="K2" t="s">
-        <v>320</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="8" t="s">
-        <v>186</v>
+      <c r="A3" t="s">
+        <v>190</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>192</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>189</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>194</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="15.75">
       <c r="A4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>194</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75">
-      <c r="A5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5" t="s">
         <v>190</v>
       </c>
-      <c r="J5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30">
       <c r="A6" s="5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>203</v>
+      </c>
       <c r="H6" s="10"/>
       <c r="I6" t="s">
-        <v>190</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30">
-      <c r="A7" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>96</v>
+        <v>204</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" ht="45">
+      <c r="A7" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" t="s">
-        <v>204</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7" s="10"/>
+        <v>192</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="1"/>
+      <c r="J7" t="s">
+        <v>194</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="45">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I8" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="J8" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="1"/>
-      <c r="J8" t="s">
-        <v>194</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="45">
-      <c r="A9" t="s">
-        <v>207</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="I9" t="s">
-        <v>205</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>211</v>
-      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>54</v>
@@ -4134,23 +4161,19 @@
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="1"/>
+      <c r="G10" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="J10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>54</v>
@@ -4162,68 +4185,72 @@
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>54</v>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>325</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30">
-      <c r="A13" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="C13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>323</v>
-      </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13" t="s">
+        <v>312</v>
+      </c>
       <c r="J13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -4235,22 +4262,22 @@
         <v>1</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="s">
         <v>312</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="31.5">
       <c r="A15" t="s">
-        <v>328</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>329</v>
+        <v>332</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>333</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
@@ -4258,26 +4285,26 @@
       <c r="D15" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>330</v>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>334</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>312</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>331</v>
+        <v>335</v>
+      </c>
+      <c r="J15" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="31.5">
       <c r="A16" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -4289,76 +4316,49 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
         <v>335</v>
       </c>
       <c r="J16" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="31.5">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>337</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>341</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>339</v>
-      </c>
-      <c r="H17"/>
-      <c r="I17" t="s">
-        <v>335</v>
-      </c>
-      <c r="J17" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
-        <v>341</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>344</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J17" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="K18" s="8"/>
+      <c r="K17" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="I9" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
+    <hyperlink ref="I6" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
+    <hyperlink ref="I8" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-899"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified test cases into post search
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="346">
   <si>
     <t>API</t>
   </si>
@@ -847,9 +847,6 @@
     <t>hits.hits._id||hits.hits.fields.title||hits.hits.fields.abstract||hits.hits.fields.source</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>OPQA-1315</t>
   </si>
   <si>
@@ -970,18 +967,12 @@
     <t>POST</t>
   </si>
   <si>
-    <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
-  </si>
-  <si>
     <t>{"title":"Creating Post For API Search Testing","content":"This post is creating for search testing"}</t>
   </si>
   <si>
     <t>Verify that to search posts by passing title</t>
   </si>
   <si>
-    <t>status=200||userId=(SYS_USER1)||found=true</t>
-  </si>
-  <si>
     <t>id||title||content</t>
   </si>
   <si>
@@ -991,9 +982,6 @@
     <t>Verify that get user profile information</t>
   </si>
   <si>
-    <t>/users/user/(SYS_USER1)</t>
-  </si>
-  <si>
     <t>firstName||lastName||primaryInstitution</t>
   </si>
   <si>
@@ -1057,10 +1045,19 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>X-1P-User=(SYS_USER1)</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||id=(OPQA-360_id)</t>
+    <t>X-1P-User=(SYS_USER3)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER3)||found=true</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER3)||id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER3)</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1546,31 +1543,31 @@
     </row>
     <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" t="s">
         <v>312</v>
-      </c>
-      <c r="B2" t="s">
-        <v>313</v>
       </c>
       <c r="C2" t="s">
         <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" t="s">
         <v>314</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="F2" t="s">
-        <v>316</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" t="s">
+        <v>342</v>
+      </c>
+      <c r="K2" t="s">
         <v>317</v>
-      </c>
-      <c r="J2" t="s">
-        <v>319</v>
-      </c>
-      <c r="K2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2201,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2551,16 +2548,13 @@
       <c r="K12" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="L12" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -2573,22 +2567,19 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>279</v>
-      </c>
       <c r="K13" s="5"/>
-      <c r="L13" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -2601,22 +2592,19 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>283</v>
-      </c>
       <c r="K14" s="5"/>
-      <c r="L14" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>285</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
@@ -2629,22 +2617,19 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>287</v>
-      </c>
       <c r="K15" s="5"/>
-      <c r="L15" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>288</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>289</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -2657,22 +2642,19 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="30">
+      <c r="A17" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>293</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>54</v>
@@ -2685,22 +2667,19 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>297</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>54</v>
@@ -2713,22 +2692,19 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>301</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
@@ -2741,22 +2717,19 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="45">
+      <c r="A20" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="K19" s="5"/>
-      <c r="L19" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>305</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>54</v>
@@ -2769,22 +2742,19 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="K20" s="5"/>
-      <c r="L20" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="30">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>309</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>54</v>
@@ -2797,15 +2767,12 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>311</v>
-      </c>
       <c r="K21" s="5"/>
-      <c r="L21" t="s">
-        <v>275</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3868,8 +3835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3998,6 +3965,7 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
+      <c r="H4"/>
       <c r="I4" t="s">
         <v>190</v>
       </c>
@@ -4111,6 +4079,7 @@
       <c r="G8" s="6" t="s">
         <v>210</v>
       </c>
+      <c r="H8"/>
       <c r="I8" t="s">
         <v>205</v>
       </c>
@@ -4164,6 +4133,7 @@
       <c r="G10" s="6" t="s">
         <v>217</v>
       </c>
+      <c r="H10"/>
       <c r="J10" s="1" t="s">
         <v>15</v>
       </c>
@@ -4187,22 +4157,23 @@
       <c r="G11" s="6" t="s">
         <v>220</v>
       </c>
+      <c r="H11"/>
       <c r="J11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C12" t="s">
         <v>134</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>323</v>
+        <v>345</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
@@ -4215,15 +4186,15 @@
         <v>15</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -4235,22 +4206,22 @@
         <v>1</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -4262,22 +4233,22 @@
         <v>1</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="31.5">
       <c r="A15" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
@@ -4289,22 +4260,22 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="J15" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="31.5">
       <c r="A16" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -4316,42 +4287,42 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="J16" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>343</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>345</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K17" s="8"/>
     </row>

</xml_diff>

<commit_message>
Fixed failing test cases in 1P Search
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -403,9 +403,6 @@
     <t>/people/details/(OPQA-434_hits.hits._id)</t>
   </si>
   <si>
-    <t>?query=Project&amp;size=1&amp;fields=fullrecord.summary.contenttype</t>
-  </si>
-  <si>
     <t>status=200||_type=people||_id=(OPQA-434_hits.hits._id)||_source.authors=Project</t>
   </si>
   <si>
@@ -415,9 +412,6 @@
     <t>Verify that user is able to search for profiles with first name</t>
   </si>
   <si>
-    <t>?query=Project&amp;size=1</t>
-  </si>
-  <si>
     <t>OPQA-501</t>
   </si>
   <si>
@@ -1058,6 +1052,12 @@
   </si>
   <si>
     <t>/users/user/(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>?query=Project&amp;size=1&amp;fields=fullrecord.summary.contenttype&amp;sort=loadtime:desc</t>
+  </si>
+  <si>
+    <t>?query=Project&amp;size=1&amp;sort=loadtime:desc</t>
   </si>
 </sst>
 </file>
@@ -1543,31 +1543,31 @@
     </row>
     <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C2" t="s">
         <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" t="s">
+        <v>339</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="E2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F2" t="s">
-        <v>341</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" t="s">
+        <v>340</v>
+      </c>
+      <c r="K2" t="s">
         <v>315</v>
-      </c>
-      <c r="J2" t="s">
-        <v>342</v>
-      </c>
-      <c r="K2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1959,7 +1959,7 @@
         <v>68</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>54</v>
@@ -1986,7 +1986,7 @@
         <v>69</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>54</v>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2013,7 +2013,7 @@
         <v>70</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2452,7 +2452,7 @@
         <v>118</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>54</v>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2491,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>15</v>
@@ -2515,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>15</v>
@@ -2524,10 +2524,10 @@
     </row>
     <row r="12" spans="1:12" ht="60">
       <c r="A12" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>54</v>
@@ -2540,21 +2540,21 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -2567,19 +2567,19 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -2592,19 +2592,19 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
@@ -2617,19 +2617,19 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -2642,19 +2642,19 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" ht="30">
       <c r="A17" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>54</v>
@@ -2667,19 +2667,19 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>54</v>
@@ -2692,19 +2692,19 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
@@ -2717,19 +2717,19 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="45">
       <c r="A20" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>54</v>
@@ -2742,19 +2742,19 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>54</v>
@@ -2767,10 +2767,10 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K21" s="5"/>
     </row>
@@ -2850,10 +2850,10 @@
     </row>
     <row r="2" spans="1:12" ht="31.5">
       <c r="A2" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
@@ -2866,34 +2866,34 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1"/>
@@ -2906,16 +2906,16 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
@@ -2930,7 +2930,7 @@
         <v>94</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>96</v>
@@ -2959,7 +2959,7 @@
         <v>99</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>96</v>
@@ -2985,16 +2985,16 @@
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
@@ -3014,50 +3014,50 @@
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -3068,23 +3068,23 @@
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -3095,22 +3095,22 @@
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="1" t="s">
@@ -3119,22 +3119,22 @@
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H12"/>
       <c r="J12" s="1" t="s">
@@ -3143,23 +3143,23 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="1"/>
@@ -3167,82 +3167,82 @@
         <v>15</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="1"/>
@@ -3250,82 +3250,82 @@
         <v>15</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30">
       <c r="A17" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>262</v>
       </c>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="A18" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H18"/>
       <c r="J18" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30">
       <c r="A19" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H19"/>
       <c r="J19" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75">
@@ -3366,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L17"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="G34" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="5" t="s">
-        <v>127</v>
+        <v>344</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
@@ -3472,15 +3472,15 @@
         <v>122</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>54</v>
@@ -3492,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>345</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>15</v>
@@ -3503,16 +3503,16 @@
     </row>
     <row r="5" spans="1:12" ht="31.5">
       <c r="A5" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -3521,19 +3521,19 @@
       <c r="G5" s="1"/>
       <c r="H5" s="5"/>
       <c r="I5" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="31.5">
       <c r="A6" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>54</v>
@@ -3545,7 +3545,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>15</v>
@@ -3556,16 +3556,16 @@
     </row>
     <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
@@ -3574,19 +3574,19 @@
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
       <c r="I7" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="31.5">
       <c r="A8" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>54</v>
@@ -3598,7 +3598,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>15</v>
@@ -3609,16 +3609,16 @@
     </row>
     <row r="9" spans="1:12" ht="31.5">
       <c r="A9" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
@@ -3627,19 +3627,19 @@
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
       <c r="I9" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="31.5">
       <c r="A10" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>54</v>
@@ -3651,18 +3651,18 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>54</v>
@@ -3674,19 +3674,19 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="31.5">
       <c r="A12" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>54</v>
@@ -3698,19 +3698,19 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="31.5">
       <c r="A13" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -3722,19 +3722,19 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="47.25">
       <c r="A14" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -3746,7 +3746,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>15</v>
@@ -3754,10 +3754,10 @@
     </row>
     <row r="15" spans="1:12" ht="31.5">
       <c r="A15" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>54</v>
@@ -3769,7 +3769,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>15</v>
@@ -3777,10 +3777,10 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -3792,7 +3792,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>15</v>
@@ -3800,10 +3800,10 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>54</v>
@@ -3816,7 +3816,7 @@
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -3835,7 +3835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L17"/>
     </sheetView>
   </sheetViews>
@@ -3895,10 +3895,10 @@
     </row>
     <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
@@ -3911,39 +3911,39 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -3951,26 +3951,26 @@
     </row>
     <row r="4" spans="1:12" ht="15.75">
       <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -3978,13 +3978,13 @@
         <v>94</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>1</v>
@@ -3993,7 +3993,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>15</v>
@@ -4007,24 +4007,24 @@
         <v>99</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>104</v>
@@ -4033,28 +4033,28 @@
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="1"/>
       <c r="J7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>107</v>
@@ -4062,50 +4062,50 @@
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>210</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="1"/>
@@ -4116,22 +4116,22 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>217</v>
       </c>
       <c r="H10"/>
       <c r="J10" s="1" t="s">
@@ -4140,22 +4140,22 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="1" t="s">
@@ -4164,16 +4164,16 @@
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
@@ -4186,143 +4186,143 @@
         <v>15</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
+        <v>322</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="31.5">
       <c r="A15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>328</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>330</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J15" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="31.5">
       <c r="A16" t="s">
+        <v>331</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>333</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>335</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="K17" s="8"/>
     </row>

</xml_diff>

<commit_message>
Added Test cases into Search
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData.xlsx
+++ b/src/test/test-data/SearchTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="359">
   <si>
     <t>API</t>
   </si>
@@ -1058,6 +1058,45 @@
   </si>
   <si>
     <t>?query=Project&amp;size=1&amp;sort=loadtime:desc</t>
+  </si>
+  <si>
+    <t>?query=Wom?n&amp;size=5</t>
+  </si>
+  <si>
+    <t>hits.hits._id[0]||hits.hits._id[1]||hits.hits._id[2]||hits.hits._id[3]||hits.hits._id[4]</t>
+  </si>
+  <si>
+    <t>OPQA-734_1</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-734_hits.hits._id[0])</t>
+  </si>
+  <si>
+    <t>status=200&amp;&amp;{_source.title=WOMAN||_source.title=WOMEN||_source.fullrecord.abstract=WOMAN||_source.fullrecord.abstract=WOMEN||_source.keywordsplus=WOMAN||_source.keywordsplus=WOMEN||_source.keywords=WOMAN||_source.keywords=WOMEN||_source.cuid=WOMAN||_source.cuid=WOMEN||_source.conferenceinfo=WOMAN||_source.conferenceinfo=WOMEN||_source.bibissueyear=WOMAN||_source.bibissueyear=WOMEN||_source.address=WOMAN||_source.address=WOMEN||_source.addresses.suborganization=WOMAN||_source.addresses.suborganization=WOMEN||_source.addresses.organization=WOMAN||_source.addresses.organization=WOMEN||_source.identifiersxml=WOMAN||_source.identifiersxml=WOMEN||_source.fullrecord.reprintinfo.author=WOMAN||_source.fullrecord.reprintinfo.author=WOMEN||_source.itemxml==WOMAN||_source.itemxml==WOMEN}</t>
+  </si>
+  <si>
+    <t>OPQA-734_2</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-734_hits.hits._id[1])</t>
+  </si>
+  <si>
+    <t>OPQA-734_3</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-734_hits.hits._id[2])</t>
+  </si>
+  <si>
+    <t>OPQA-734_4</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-734_hits.hits._id[3])</t>
+  </si>
+  <si>
+    <t>OPQA-734_5</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-734_hits.hits._id[4])</t>
   </si>
 </sst>
 </file>
@@ -1481,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L25"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2035,7 +2074,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="45">
       <c r="A20" s="1" t="s">
         <v>71</v>
       </c>
@@ -2046,25 +2085,25 @@
         <v>54</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>346</v>
       </c>
       <c r="H20"/>
       <c r="J20" t="s">
         <v>15</v>
       </c>
-      <c r="K20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="75">
+      <c r="K20" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="135">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>348</v>
       </c>
       <c r="B21" t="s">
         <v>49</v>
@@ -2073,7 +2112,7 @@
         <v>54</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>83</v>
+        <v>349</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -2083,108 +2122,255 @@
         <v>71</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="135">
       <c r="A22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>50</v>
+        <v>351</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>12</v>
+        <v>352</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="G22" t="s">
-        <v>29</v>
-      </c>
       <c r="H22"/>
+      <c r="I22" t="s">
+        <v>71</v>
+      </c>
       <c r="J22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="60">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="135">
       <c r="A23" s="1" t="s">
-        <v>74</v>
+        <v>353</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>84</v>
+        <v>354</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="H23"/>
       <c r="I23" t="s">
-        <v>73</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="30">
+        <v>71</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="135">
       <c r="A24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>51</v>
+        <v>355</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>12</v>
+        <v>356</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="G24" t="s">
-        <v>30</v>
-      </c>
       <c r="H24"/>
+      <c r="I24" t="s">
+        <v>71</v>
+      </c>
       <c r="J24" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="120">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="135">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>357</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>85</v>
+        <v>358</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
       <c r="H25"/>
       <c r="I25" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26"/>
+      <c r="J26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="75">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27"/>
+      <c r="I27" t="s">
+        <v>71</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30">
+      <c r="A28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28"/>
+      <c r="J28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="60">
+      <c r="A29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29"/>
+      <c r="I29" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30">
+      <c r="A30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="B30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30"/>
+      <c r="J30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="120">
+      <c r="A31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31"/>
+      <c r="I31" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2196,10 +2382,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2773,6 +2959,157 @@
         <v>308</v>
       </c>
       <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="45">
+      <c r="A22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>346</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="135">
+      <c r="A23" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23"/>
+      <c r="I23" t="s">
+        <v>71</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="1:11" ht="135">
+      <c r="A24" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24"/>
+      <c r="I24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="K24"/>
+    </row>
+    <row r="25" spans="1:11" ht="135">
+      <c r="A25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25"/>
+      <c r="I25" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="K25"/>
+    </row>
+    <row r="26" spans="1:11" ht="135">
+      <c r="A26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26"/>
+      <c r="I26" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="1:11" ht="135">
+      <c r="A27" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27"/>
+      <c r="I27" t="s">
+        <v>71</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="K27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3366,8 +3703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="G34" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>